<commit_message>
finaliza jornada QH 17-12-2014
</commit_message>
<xml_diff>
--- a/app/rep/Mexico HS Code 21.xlsx
+++ b/app/rep/Mexico HS Code 21.xlsx
@@ -132,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -144,6 +144,12 @@
     </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="49" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,7 +454,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -506,44 +512,44 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>2012</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>15518736.32</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>14447812.13</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>-1070924.19</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>2013</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>19015241.27</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>13943063.81</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>-5072177.46</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>2014</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>16787467.34</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>12292793.74</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>-4494673.6</v>
       </c>
     </row>

</xml_diff>